<commit_message>
Support Burn Grading Forest
* Add XLSForm `inst/odk/BurnGradingForest.xlsx`
* Deploy BurnGradingForest to test server, capture and download example data, close #12
* Add data("bgf") to use in tests, examples, vignettes, close #13
* Change extract_grading to handle dashes `-` as NA, #8
* Add `calculate_ozcbi_forest`: uses new formula for Forest OzCBI and variable names from data("bgf"), close #8
* Add `add_ozcbi_forest`, close #10
* Update media files for vignette: delete old photos, add new photos
* Update tests
* Update examples
* Update vignettes to use data("bgf"), close #13
* Update GitHub actions
</commit_message>
<xml_diff>
--- a/inst/odk/BurnGradingForest.xlsx
+++ b/inst/odk/BurnGradingForest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fmayer\projects\rOzCBI\inst\odk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F43C1DC-BF5A-48EE-AE71-2410DE0662D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4152131D-EAD2-4DB4-BD2F-D44119E1DDFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17190" yWindow="-18120" windowWidth="29040" windowHeight="18240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17310" yWindow="-18000" windowWidth="14400" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="settings" sheetId="3" r:id="rId3"/>
     <sheet name="warnings" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0" refMode="R1C1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -1261,12 +1261,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="49.4140625" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" customWidth="1"/>
+    <col min="3" max="3" width="37.1640625" customWidth="1"/>
     <col min="8" max="8" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2019,7 +2022,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A2:G6 A8:G54 A7 C7:G7 A1:B1 E1 G1" numberStoredAsText="1"/>
+    <ignoredError sqref="A2:G6 A8:G47 A7 C7:G7 A1:B1 E1 G1 A49:G54 A48:C48 E48:G48" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -2033,6 +2036,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="41.4140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -3520,7 +3526,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>

</xml_diff>